<commit_message>
penambahan DHS paling bawah
</commit_message>
<xml_diff>
--- a/database/database_apollo_class.xlsx
+++ b/database/database_apollo_class.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ptorbitventurainodnesia-my.sharepoint.com/personal/rizal_orbitfutureacademy_sch_id/Documents/Afrizal Meka/Project Pribadi/aplikasi-cek-nilai-posttest/database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="553" documentId="8_{05BD83B4-5392-4445-AAC5-12E6CFF7250D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{25E93AB7-7AAC-D249-8C4D-303B6F8145B8}"/>
+  <xr:revisionPtr revIDLastSave="555" documentId="8_{05BD83B4-5392-4445-AAC5-12E6CFF7250D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D6178586-6DC0-5148-AA63-4D78CAE2F5AB}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16440" activeTab="7" xr2:uid="{D1024BA5-EBE1-5D48-A10D-EB249C632C01}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16440" activeTab="6" xr2:uid="{D1024BA5-EBE1-5D48-A10D-EB249C632C01}"/>
   </bookViews>
   <sheets>
     <sheet name="intro_ai" sheetId="1" r:id="rId1"/>
@@ -9671,9 +9671,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE923BF7-4920-F34C-8CDD-3755F3BF580F}">
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I22" sqref="I22"/>
+      <selection pane="topRight" activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9888,7 +9888,7 @@
         <v>8</v>
       </c>
       <c r="B7" s="17">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="C7" s="17">
         <v>100</v>
@@ -10020,7 +10020,7 @@
         <v>12</v>
       </c>
       <c r="B11" s="17">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="C11" s="17">
         <v>100</v>
@@ -10726,7 +10726,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D92A33F5-6D91-C94E-BA3D-71D5E4D8A34B}">
   <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="J33" sqref="J33"/>
     </sheetView>

</xml_diff>

<commit_message>
bug final score intro to ai
</commit_message>
<xml_diff>
--- a/database/database_apollo_class.xlsx
+++ b/database/database_apollo_class.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ptorbitventurainodnesia-my.sharepoint.com/personal/rizal_orbitfutureacademy_sch_id/Documents/Afrizal Meka/Project Pribadi/aplikasi-cek-nilai-posttest/database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="562" documentId="8_{05BD83B4-5392-4445-AAC5-12E6CFF7250D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2874FDC7-DD68-884D-9D93-8B9E2D2F739A}"/>
+  <xr:revisionPtr revIDLastSave="563" documentId="8_{05BD83B4-5392-4445-AAC5-12E6CFF7250D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{16EB7084-34CC-A24F-BDBF-532E70000DB8}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16440" activeTab="2" xr2:uid="{D1024BA5-EBE1-5D48-A10D-EB249C632C01}"/>
+    <workbookView xWindow="14520" yWindow="0" windowWidth="14280" windowHeight="18000" activeTab="4" xr2:uid="{D1024BA5-EBE1-5D48-A10D-EB249C632C01}"/>
   </bookViews>
   <sheets>
     <sheet name="intro_ai" sheetId="1" r:id="rId1"/>
@@ -938,8 +938,8 @@
   <dimension ref="A1:P32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G22" sqref="G22"/>
+      <pane xSplit="1" topLeftCell="M1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1046,8 +1046,8 @@
       <c r="N2" s="12">
         <v>70</v>
       </c>
-      <c r="O2" s="13">
-        <v>83.25</v>
+      <c r="O2" s="4">
+        <v>86.5</v>
       </c>
       <c r="P2" s="14" t="str">
         <f t="shared" ref="P2:P32" si="0">IF(O2&gt;=80,"A",IF(O2&gt;=70,"B",IF(O2&gt;=50,"C",IF(O2&gt;=40,"D","E"))))</f>
@@ -1097,12 +1097,12 @@
       <c r="N3" s="12">
         <v>60</v>
       </c>
-      <c r="O3" s="13">
-        <v>74.5</v>
+      <c r="O3" s="4">
+        <v>82.2</v>
       </c>
       <c r="P3" s="14" t="str">
         <f t="shared" si="0"/>
-        <v>B</v>
+        <v>A</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
@@ -1148,8 +1148,8 @@
       <c r="N4" s="12">
         <v>70</v>
       </c>
-      <c r="O4" s="13">
-        <v>90.69</v>
+      <c r="O4" s="4">
+        <v>87.4</v>
       </c>
       <c r="P4" s="14" t="str">
         <f t="shared" si="0"/>
@@ -1199,12 +1199,12 @@
       <c r="N5" s="12">
         <v>60</v>
       </c>
-      <c r="O5" s="13">
-        <v>64.06</v>
+      <c r="O5" s="4">
+        <v>83.1</v>
       </c>
       <c r="P5" s="14" t="str">
         <f t="shared" si="0"/>
-        <v>C</v>
+        <v>A</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
@@ -1250,8 +1250,8 @@
       <c r="N6" s="12">
         <v>80</v>
       </c>
-      <c r="O6" s="13">
-        <v>82.13</v>
+      <c r="O6" s="4">
+        <v>91.7</v>
       </c>
       <c r="P6" s="14" t="str">
         <f t="shared" si="0"/>
@@ -1301,12 +1301,12 @@
       <c r="N7" s="12">
         <v>50</v>
       </c>
-      <c r="O7" s="13">
-        <v>69.63</v>
+      <c r="O7" s="4">
+        <v>78.5</v>
       </c>
       <c r="P7" s="14" t="str">
         <f t="shared" si="0"/>
-        <v>C</v>
+        <v>B</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
@@ -1352,8 +1352,8 @@
       <c r="N8" s="12">
         <v>90</v>
       </c>
-      <c r="O8" s="13">
-        <v>92.13</v>
+      <c r="O8" s="4">
+        <v>95.1</v>
       </c>
       <c r="P8" s="14" t="str">
         <f t="shared" si="0"/>
@@ -1403,12 +1403,12 @@
       <c r="N9" s="12">
         <v>60</v>
       </c>
-      <c r="O9" s="13">
-        <v>71.31</v>
+      <c r="O9" s="4">
+        <v>83.7</v>
       </c>
       <c r="P9" s="14" t="str">
         <f t="shared" si="0"/>
-        <v>B</v>
+        <v>A</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
@@ -1454,12 +1454,12 @@
       <c r="N10" s="12">
         <v>80</v>
       </c>
-      <c r="O10" s="13">
-        <v>69.44</v>
+      <c r="O10" s="4">
+        <v>90.5</v>
       </c>
       <c r="P10" s="14" t="str">
         <f t="shared" si="0"/>
-        <v>C</v>
+        <v>A</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
@@ -1505,12 +1505,12 @@
       <c r="N11" s="12">
         <v>70</v>
       </c>
-      <c r="O11" s="13">
-        <v>65</v>
+      <c r="O11" s="4">
+        <v>87.1</v>
       </c>
       <c r="P11" s="14" t="str">
         <f t="shared" si="0"/>
-        <v>C</v>
+        <v>A</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
@@ -1556,8 +1556,8 @@
       <c r="N12" s="12">
         <v>80</v>
       </c>
-      <c r="O12" s="13">
-        <v>90.31</v>
+      <c r="O12" s="4">
+        <v>91.1</v>
       </c>
       <c r="P12" s="14" t="str">
         <f t="shared" si="0"/>
@@ -1607,12 +1607,12 @@
       <c r="N13" s="12">
         <v>80</v>
       </c>
-      <c r="O13" s="13">
-        <v>66.63</v>
+      <c r="O13" s="4">
+        <v>91.4</v>
       </c>
       <c r="P13" s="14" t="str">
         <f t="shared" si="0"/>
-        <v>C</v>
+        <v>A</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
@@ -1658,12 +1658,12 @@
       <c r="N14" s="12">
         <v>50</v>
       </c>
-      <c r="O14" s="13">
-        <v>65.56</v>
+      <c r="O14" s="4">
+        <v>78.5</v>
       </c>
       <c r="P14" s="14" t="str">
         <f t="shared" si="0"/>
-        <v>C</v>
+        <v>B</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
@@ -1709,12 +1709,12 @@
       <c r="N15" s="12">
         <v>90</v>
       </c>
-      <c r="O15" s="13">
-        <v>77.81</v>
+      <c r="O15" s="4">
+        <v>95.4</v>
       </c>
       <c r="P15" s="14" t="str">
         <f t="shared" si="0"/>
-        <v>B</v>
+        <v>A</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
@@ -1760,12 +1760,12 @@
       <c r="N16" s="12">
         <v>80</v>
       </c>
-      <c r="O16" s="13">
-        <v>52.25</v>
+      <c r="O16" s="4">
+        <v>91.1</v>
       </c>
       <c r="P16" s="14" t="str">
         <f t="shared" si="0"/>
-        <v>C</v>
+        <v>A</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.2">
@@ -1811,12 +1811,12 @@
       <c r="N17" s="12">
         <v>50</v>
       </c>
-      <c r="O17" s="13">
-        <v>80.63</v>
+      <c r="O17" s="4">
+        <v>79.099999999999994</v>
       </c>
       <c r="P17" s="14" t="str">
         <f t="shared" si="0"/>
-        <v>A</v>
+        <v>B</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.2">
@@ -1862,8 +1862,8 @@
       <c r="N18" s="12">
         <v>90</v>
       </c>
-      <c r="O18" s="13">
-        <v>91.63</v>
+      <c r="O18" s="4">
+        <v>95.7</v>
       </c>
       <c r="P18" s="14" t="str">
         <f t="shared" si="0"/>
@@ -1913,8 +1913,8 @@
       <c r="N19" s="12">
         <v>90</v>
       </c>
-      <c r="O19" s="13">
-        <v>83.25</v>
+      <c r="O19" s="4">
+        <v>95.4</v>
       </c>
       <c r="P19" s="14" t="str">
         <f t="shared" si="0"/>
@@ -1964,8 +1964,8 @@
       <c r="N20" s="12">
         <v>100</v>
       </c>
-      <c r="O20" s="13">
-        <v>82.69</v>
+      <c r="O20" s="4">
+        <v>99.1</v>
       </c>
       <c r="P20" s="14" t="str">
         <f t="shared" si="0"/>
@@ -2015,8 +2015,8 @@
       <c r="N21" s="12">
         <v>80</v>
       </c>
-      <c r="O21" s="13">
-        <v>89.38</v>
+      <c r="O21" s="4">
+        <v>91.4</v>
       </c>
       <c r="P21" s="14" t="str">
         <f t="shared" si="0"/>
@@ -2066,12 +2066,12 @@
       <c r="N22" s="12">
         <v>90</v>
       </c>
-      <c r="O22" s="13">
-        <v>73.56</v>
+      <c r="O22" s="4">
+        <v>95.4</v>
       </c>
       <c r="P22" s="14" t="str">
         <f t="shared" si="0"/>
-        <v>B</v>
+        <v>A</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.2">
@@ -2117,8 +2117,8 @@
       <c r="N23" s="12">
         <v>70</v>
       </c>
-      <c r="O23" s="13">
-        <v>81.56</v>
+      <c r="O23" s="4">
+        <v>87.4</v>
       </c>
       <c r="P23" s="14" t="str">
         <f t="shared" si="0"/>
@@ -2168,12 +2168,12 @@
       <c r="N24" s="12">
         <v>50</v>
       </c>
-      <c r="O24" s="13">
-        <v>89.19</v>
+      <c r="O24" s="4">
+        <v>79.400000000000006</v>
       </c>
       <c r="P24" s="14" t="str">
         <f t="shared" si="0"/>
-        <v>A</v>
+        <v>B</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.2">
@@ -2219,8 +2219,8 @@
       <c r="N25" s="12">
         <v>80</v>
       </c>
-      <c r="O25" s="13">
-        <v>83.44</v>
+      <c r="O25" s="4">
+        <v>91.1</v>
       </c>
       <c r="P25" s="14" t="str">
         <f t="shared" si="0"/>
@@ -2270,12 +2270,12 @@
       <c r="N26" s="12">
         <v>70</v>
       </c>
-      <c r="O26" s="13">
-        <v>65.56</v>
+      <c r="O26" s="4">
+        <v>87.4</v>
       </c>
       <c r="P26" s="14" t="str">
         <f t="shared" si="0"/>
-        <v>C</v>
+        <v>A</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.2">
@@ -2321,8 +2321,8 @@
       <c r="N27" s="12">
         <v>90</v>
       </c>
-      <c r="O27" s="13">
-        <v>86.19</v>
+      <c r="O27" s="4">
+        <v>95.4</v>
       </c>
       <c r="P27" s="14" t="str">
         <f t="shared" si="0"/>
@@ -2372,12 +2372,12 @@
       <c r="N28" s="12">
         <v>60</v>
       </c>
-      <c r="O28" s="13">
-        <v>73.38</v>
+      <c r="O28" s="4">
+        <v>82.5</v>
       </c>
       <c r="P28" s="14" t="str">
         <f t="shared" si="0"/>
-        <v>B</v>
+        <v>A</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.2">
@@ -2423,8 +2423,8 @@
       <c r="N29" s="12">
         <v>90</v>
       </c>
-      <c r="O29" s="13">
-        <v>86.75</v>
+      <c r="O29" s="4">
+        <v>95.4</v>
       </c>
       <c r="P29" s="14" t="str">
         <f t="shared" si="0"/>
@@ -2474,12 +2474,12 @@
       <c r="N30" s="12">
         <v>60</v>
       </c>
-      <c r="O30" s="13">
-        <v>73.38</v>
+      <c r="O30" s="4">
+        <v>83.4</v>
       </c>
       <c r="P30" s="14" t="str">
         <f t="shared" si="0"/>
-        <v>B</v>
+        <v>A</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.2">
@@ -2591,7 +2591,7 @@
   <dimension ref="A1:T33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="G1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" topLeftCell="P1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" sqref="A1:A32"/>
     </sheetView>
   </sheetViews>
@@ -4636,9 +4636,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7913E6DD-EB3B-FB44-A801-0D323E8EABCE}">
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F16" sqref="F16"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5677,7 +5677,7 @@
   <dimension ref="A1:T32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" topLeftCell="Q1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="S36" sqref="S36"/>
     </sheetView>
   </sheetViews>
@@ -7605,9 +7605,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B08BDEB-EA3E-1246-B578-6F2735C5EEF4}">
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A25" sqref="A25"/>
+      <selection pane="topRight" activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>